<commit_message>
-am Updated summoning calcs and added ki calcs to getKitFromUsr
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BCC842-E520-4E86-9BE4-D15EDC74F06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC38F496-85EC-4414-B4E5-1518357C1784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="0" windowWidth="11415" windowHeight="14280" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Task</t>
   </si>
@@ -44,13 +44,10 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Prime Battle</t>
+    <t>Super Strike</t>
   </si>
   <si>
-    <t>Turles Dokkan Event</t>
-  </si>
-  <si>
-    <t>SBR</t>
+    <t>LVE Mission</t>
   </si>
 </sst>
 </file>
@@ -402,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436DF741-E1F7-49CA-BEC1-DDAEC756EB64}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -421,25 +418,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added damage taken calculations
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72530B5-A933-4487-9315-06643E52BCA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68B57C6-E981-43F0-9BA0-083071733946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Task</t>
   </si>
@@ -52,21 +52,25 @@
   <si>
     <t>STR Whis</t>
   </si>
-  <si>
-    <t>Dokkan Medals for Baby</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436DF741-E1F7-49CA-BEC1-DDAEC756EB64}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -424,11 +429,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>2</v>
@@ -442,7 +442,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished import from dokkanUnit.py
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68B57C6-E981-43F0-9BA0-083071733946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D691EEA-DB1F-45A3-BCFC-4B57F5A9F14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Task</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>STR Whis</t>
+  </si>
+  <si>
+    <t>Don Kai's Event</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -429,6 +432,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Added additional supers to ki sphere dependent buffs
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D691EEA-DB1F-45A3-BCFC-4B57F5A9F14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDF5EF0-1B58-43D1-9AA8-C49E03D3EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
@@ -36,24 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Task</t>
   </si>
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>Treasures</t>
-  </si>
-  <si>
-    <t>Int god goku</t>
-  </si>
-  <si>
-    <t>STR Whis</t>
-  </si>
-  <si>
-    <t>Don Kai's Event</t>
   </si>
 </sst>
 </file>
@@ -416,7 +404,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -432,24 +420,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add multi-turn buffs for ki-sphere buffs
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDF5EF0-1B58-43D1-9AA8-C49E03D3EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F76A65-DA0F-4FDF-BF13-60AFC5D35DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
@@ -36,12 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Task</t>
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>Chocolate Treasures</t>
+  </si>
+  <si>
+    <t>Water Seal Key Treasures</t>
+  </si>
+  <si>
+    <t>Kachi Katchin Treasures</t>
   </si>
 </sst>
 </file>
@@ -404,7 +413,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -420,6 +429,21 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add abiltiy after guard activated
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9632B9-F92B-4B25-9566-1F67EFC4C819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A076D07-72C0-4BBB-9515-120A29729175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
@@ -36,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Task</t>
   </si>
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>Kachi Katchin Treasures</t>
-  </si>
-  <si>
-    <t>Ultimate Speed Battle</t>
   </si>
 </sst>
 </file>
@@ -410,7 +404,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -426,16 +420,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Cap heal to 100%
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA130836-3324-448F-89F9-1CDE40365101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8461575E-385C-429A-81F7-DE4E4E015EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
@@ -404,7 +404,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Remove old threshold abilities
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8461575E-385C-429A-81F7-DE4E4E015EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C461C6D3-BCE6-4281-BDF0-C20D1A18D1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AD712AF9-C8EA-4C20-96A3-BDC9D00093DF}"/>
   </bookViews>
@@ -404,7 +404,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A3" sqref="A3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>